<commit_message>
Switched LED footprint and fixed row traces
- Switched LED footprints from 0402 to 0603 to reduce assembly cost
- Added back row traces that were accidentally removed in an earlier commit
</commit_message>
<xml_diff>
--- a/Fabrication/BoM.xlsx
+++ b/Fabrication/BoM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan\Documents\GitHub\BusinessCard\Fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{133C7661-478D-7E4E-909A-40DAC11E6D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7E2A2D-69F3-4756-894D-895D034B15BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="16800" windowHeight="19100" xr2:uid="{125DEEBA-1ADD-3248-B2D6-B318EBD508C6}"/>
+    <workbookView xWindow="38280" yWindow="3375" windowWidth="29040" windowHeight="15720" xr2:uid="{125DEEBA-1ADD-3248-B2D6-B318EBD508C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,12 +50,6 @@
     <t>JLCPCB Part #</t>
   </si>
   <si>
-    <t>C1 C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>D2-145</t>
   </si>
   <si>
@@ -101,25 +95,31 @@
     <t>C1525</t>
   </si>
   <si>
-    <t>C307423</t>
-  </si>
-  <si>
-    <t>C88330</t>
-  </si>
-  <si>
     <t>C8734</t>
   </si>
   <si>
-    <t>C25531</t>
-  </si>
-  <si>
-    <t>C25543</t>
-  </si>
-  <si>
-    <t>C25151</t>
-  </si>
-  <si>
     <t>C191023</t>
+  </si>
+  <si>
+    <t>C23733</t>
+  </si>
+  <si>
+    <t>C25744</t>
+  </si>
+  <si>
+    <t>C11702</t>
+  </si>
+  <si>
+    <t>C25091</t>
+  </si>
+  <si>
+    <t>C1 C2 C3 C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C2286</t>
   </si>
 </sst>
 </file>
@@ -493,16 +493,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E586EF-563B-F549-B7B6-40B7D6EB3D62}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,26 +516,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>402</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>402</v>
@@ -544,88 +544,88 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>603</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
-      </c>
-      <c r="C4">
-        <v>402</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
       <c r="C6">
         <v>402</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>402</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>220</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>402</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>